<commit_message>
Updated part list for wifi version
</commit_message>
<xml_diff>
--- a/LipSync_Mini_Wifi_BOM.xlsx
+++ b/LipSync_Mini_Wifi_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milad\Development\LipSync-Modified\LipSync-Mini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DBBC13-082D-4518-9B02-DCAAAF89FD24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34FD592-CD13-49B8-96B0-8C5A6C828646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="11140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="249">
   <si>
     <t>Qty</t>
   </si>
@@ -777,6 +777,9 @@
   </si>
   <si>
     <t>S7107-ND</t>
+  </si>
+  <si>
+    <t>8 Position Header Connector Through Hole</t>
   </si>
 </sst>
 </file>
@@ -1645,7 +1648,7 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1810,6 +1813,9 @@
       </c>
       <c r="B5" t="s">
         <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>248</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>

</xml_diff>